<commit_message>
xong. deo lam nua
</commit_message>
<xml_diff>
--- a/app/static/temp/bao_cao_thang_12.xlsx
+++ b/app/static/temp/bao_cao_thang_12.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,10 +460,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-12-06</t>
-        </is>
+      <c r="A2" s="2" t="n">
+        <v>45632</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -468,14 +470,12 @@
         <v>145000</v>
       </c>
       <c r="D2" t="n">
-        <v>0.141</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-12-19</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>45645</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -484,14 +484,12 @@
         <v>180000</v>
       </c>
       <c r="D3" t="n">
-        <v>0.176</v>
+        <v>0.153</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-12-21</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>45647</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -500,20 +498,34 @@
         <v>200000</v>
       </c>
       <c r="D4" t="n">
-        <v>0.195</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="n">
+        <v>45651</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>220000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
-        <v>1025000</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>1175000</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>